<commit_message>
Commit the code for WebElement Implementatio
Commit the code for WebElement Implementatio
</commit_message>
<xml_diff>
--- a/Resources/TestData/B4C_TestData.xlsx
+++ b/Resources/TestData/B4C_TestData.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="76">
   <si>
     <t>Feature</t>
   </si>
@@ -232,28 +232,28 @@
     <t>Producer_Code</t>
   </si>
   <si>
-    <t>Enigma Fire &amp; Casualty</t>
-  </si>
-  <si>
-    <t>dfgd</t>
-  </si>
-  <si>
     <t>Account_ID</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>OS3</t>
-  </si>
-  <si>
-    <t>7912773240</t>
-  </si>
-  <si>
-    <t>Demo3</t>
-  </si>
-  <si>
-    <t>4890575779</t>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>Demo</t>
+  </si>
+  <si>
+    <t>ACV Property Insurance</t>
+  </si>
+  <si>
+    <t>301-008578 ACV Property Insurance</t>
+  </si>
+  <si>
+    <t>UserStory</t>
+  </si>
+  <si>
+    <t>4025692771</t>
   </si>
 </sst>
 </file>
@@ -679,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -706,7 +706,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>2</v>
@@ -750,8 +750,8 @@
       <c r="P1" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="Q1" s="11" t="s">
-        <v>70</v>
+      <c r="Q1" s="3" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
@@ -775,11 +775,11 @@
       </c>
       <c r="G2" s="5" t="str">
         <f>G3</f>
-        <v>OS3</v>
+        <v>Team</v>
       </c>
       <c r="H2" s="5" t="str">
         <f>H3</f>
-        <v>Demo3</v>
+        <v>Demo</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
@@ -789,7 +789,7 @@
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
+      <c r="Q2" s="6"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
@@ -811,10 +811,10 @@
         <v>1</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>9</v>
@@ -835,12 +835,12 @@
         <v>65</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q3" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q3" s="6" t="s">
         <v>75</v>
       </c>
     </row>
@@ -854,7 +854,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:G3"/>
+      <selection activeCell="A2" sqref="A2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -991,7 +991,7 @@
   <dimension ref="A1:AA2"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="J1" sqref="J1:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1129,7 +1129,7 @@
         <v>34</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J2" s="6" t="b">
         <v>0</v>

</xml_diff>